<commit_message>
"Journal de travail" and it's csv version done
</commit_message>
<xml_diff>
--- a/JournalTravail/Journal_Travail_Muaremi.xlsx
+++ b/JournalTravail/Journal_Travail_Muaremi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
   <si>
     <t>Date</t>
   </si>
@@ -60,9 +60,6 @@
     <t>Rédaction du modèle de Gant sous Excel, ainsi que des répartitions des heures</t>
   </si>
   <si>
-    <t>03.03.2018 -</t>
-  </si>
-  <si>
     <t>Mise à jour des répartitions des heures</t>
   </si>
   <si>
@@ -84,15 +81,9 @@
     <t>Réunion : Définir les tâches à réaliser des vacances</t>
   </si>
   <si>
-    <t>vacances</t>
-  </si>
-  <si>
     <t>Réunion choix de proposition projet</t>
   </si>
   <si>
-    <t>Début du projet</t>
-  </si>
-  <si>
     <t>Réunion avancement après vacances</t>
   </si>
   <si>
@@ -111,9 +102,6 @@
     <t>Implémentation de la base de données</t>
   </si>
   <si>
-    <t>Ajout de méthodes sur la base de données. call java -&gt; procedure MySQL</t>
-  </si>
-  <si>
     <t>Création des classes pour la communication Java - MySQL</t>
   </si>
   <si>
@@ -129,10 +117,19 @@
     <t>Réunion du petit groupe : Restructuration du projet</t>
   </si>
   <si>
-    <t>ascencion</t>
-  </si>
-  <si>
-    <t>Lundi de truc</t>
+    <t>Projet</t>
+  </si>
+  <si>
+    <t>Call Java sur les méthodes de la base de données</t>
+  </si>
+  <si>
+    <t>Ajout de méthodes sur la base de données.</t>
+  </si>
+  <si>
+    <t>Correction de bug java sur les Call des méthodes SQL</t>
+  </si>
+  <si>
+    <t>Correction de bug sur les méthodes SQL et Java</t>
   </si>
 </sst>
 </file>
@@ -142,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,7 +179,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -243,9 +246,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -258,9 +258,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -276,23 +273,29 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -602,438 +605,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="4"/>
+    <col min="1" max="1" width="8.85546875" style="3"/>
     <col min="2" max="2" width="52.5703125" style="15" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" style="10"/>
-    <col min="4" max="5" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="4"/>
+    <col min="3" max="3" width="8.85546875" style="8"/>
+    <col min="4" max="5" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="14"/>
-      <c r="C1" s="9"/>
-    </row>
-    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43153</v>
       </c>
-      <c r="B5" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="12">
+      <c r="B5" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43154</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43160</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="8" t="s">
+      <c r="B7" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>43162</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43165</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43167</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="12">
+      <c r="B10" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43167</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43174</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="12">
-        <v>2</v>
-      </c>
-      <c r="D12" s="19">
-        <v>43174</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="10">
+        <v>2</v>
+      </c>
+      <c r="D12" s="12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43176</v>
       </c>
-      <c r="B13" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="12">
+      <c r="B13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="10">
         <v>2.5</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43179</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="12"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>43183</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43186</v>
       </c>
-      <c r="B16" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="12"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>43189</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43193</v>
       </c>
-      <c r="B18" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="12">
-        <v>2</v>
-      </c>
-      <c r="D18" s="19">
-        <v>43192</v>
-      </c>
-      <c r="E18" s="19">
-        <v>43198</v>
-      </c>
-      <c r="F18" s="4" t="s">
+      <c r="B18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43197</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43200</v>
+      </c>
+      <c r="B20" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="4" t="s">
+      <c r="C20" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43204</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43205</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43208</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43209</v>
+      </c>
+      <c r="B24" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="10">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43215</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>43223</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43228</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43233</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43235</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="10">
+        <v>4</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43238</v>
+      </c>
+      <c r="B30" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>43200</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="12"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>43208</v>
-      </c>
-      <c r="B24" s="18" t="s">
+      <c r="C30" s="10">
         <v>6</v>
       </c>
-      <c r="C24" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>43209</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="12">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="12"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>43223</v>
-      </c>
-      <c r="B27" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="12"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="12"/>
-    </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>43228</v>
-      </c>
-      <c r="B30" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="12">
-        <v>2</v>
-      </c>
-      <c r="D30" s="19">
-        <v>43230</v>
-      </c>
-      <c r="E30" s="19">
-        <v>43231</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>43233</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="12"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43239</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>43235</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C32" s="12"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19">
-        <v>43241</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>37</v>
+        <v>43240</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="10">
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>43238</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="12">
-        <v>6</v>
+        <v>43241</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C33" s="10">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>43241</v>
-      </c>
-      <c r="B34" s="18" t="s">
+      <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="12">
-        <v>2</v>
+      <c r="B34" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="10">
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="12"/>
+      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="10">
+        <v>8</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="12"/>
+      <c r="A36" s="1">
+        <v>43244</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="10">
+        <v>2</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="12"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="12"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="12"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="12"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="12"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="12"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="12"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="12"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
-        <v>43244</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C45" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="17" t="s">
+      <c r="B37" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C46" s="13">
-        <f>SUM(C5:C45)</f>
-        <v>45</v>
+      <c r="C37" s="11">
+        <f>SUM(C5:C36)</f>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Spell check for mine and added the resume for Aurélien Manalito Adrien Siu
</commit_message>
<xml_diff>
--- a/JournalTravail/Journal_Travail_Muaremi.xlsx
+++ b/JournalTravail/Journal_Travail_Muaremi.xlsx
@@ -45,48 +45,18 @@
     <t>Préparation de la présentation et présentation</t>
   </si>
   <si>
-    <t>Réunion de groupe afin de définir les tâches à faire durant la période de l'ascension</t>
-  </si>
-  <si>
     <t>Dejvid Muaremi</t>
   </si>
   <si>
     <t>Réunion de groupe</t>
   </si>
   <si>
-    <t>Changement de modèle de Gant</t>
-  </si>
-  <si>
-    <t>Rédaction du modèle de Gant sous Excel, ainsi que des répartitions des heures</t>
-  </si>
-  <si>
     <t>Mise à jour des répartitions des heures</t>
   </si>
   <si>
-    <t>Introduction du module. Constitution du groupe avec nomination d'un chef de groupe et de son remplaçant.</t>
-  </si>
-  <si>
-    <t>Feedback des propositions. Discussion pour compléter le projet choisi : DARYLL</t>
-  </si>
-  <si>
-    <t>Réunion : Refaire la planification initiale</t>
-  </si>
-  <si>
     <t>Finalisation et rendu</t>
   </si>
   <si>
-    <t>Réunion : Discuter des fonctionnalités du projet</t>
-  </si>
-  <si>
-    <t>Réunion : Définir les tâches à réaliser des vacances</t>
-  </si>
-  <si>
-    <t>Réunion choix de proposition projet</t>
-  </si>
-  <si>
-    <t>Réunion avancement après vacances</t>
-  </si>
-  <si>
     <t>Réunion durant les vacances</t>
   </si>
   <si>
@@ -102,9 +72,6 @@
     <t>Implémentation de la base de données</t>
   </si>
   <si>
-    <t>Création des classes pour la communication Java - MySQL</t>
-  </si>
-  <si>
     <t>Réunion de groupe afin de définir les dernières tâches</t>
   </si>
   <si>
@@ -114,9 +81,6 @@
     <t>Rédaction de la documentation utilisateur</t>
   </si>
   <si>
-    <t>Réunion du petit groupe : Restructuration du projet</t>
-  </si>
-  <si>
     <t>Projet</t>
   </si>
   <si>
@@ -126,10 +90,46 @@
     <t>Ajout de méthodes sur la base de données.</t>
   </si>
   <si>
-    <t>Correction de bug java sur les Call des méthodes SQL</t>
-  </si>
-  <si>
     <t>Correction de bug sur les méthodes SQL et Java</t>
+  </si>
+  <si>
+    <t>Changement de modèle de Gantt</t>
+  </si>
+  <si>
+    <t>Correction de bug Java sur les calls des méthodes SQL</t>
+  </si>
+  <si>
+    <t>Introduction du module. Constitution du groupe avec nomination d’un chef de groupe et de son remplaçant.</t>
+  </si>
+  <si>
+    <t>Réunion de groupe afin de définir les tâches à faire durant la période de l’ascension</t>
+  </si>
+  <si>
+    <t>Création des classes pour la communication Java — MySQL</t>
+  </si>
+  <si>
+    <t>Rédaction du modèle de Gantt sous Excel, ainsi que des répartitions des heures</t>
+  </si>
+  <si>
+    <t>Réunion: choix de proposition projet</t>
+  </si>
+  <si>
+    <t>Feedback des propositions. Discussion pour compléter le projet choisi: DARYLL</t>
+  </si>
+  <si>
+    <t>Réunion: Discuter des fonctionnalités du projet</t>
+  </si>
+  <si>
+    <t>Réunion: Refaire la planification initiale</t>
+  </si>
+  <si>
+    <t>Réunion: Définir les tâches à réaliser des vacances</t>
+  </si>
+  <si>
+    <t>Réunion: avancement après vacances</t>
+  </si>
+  <si>
+    <t>Réunion du petit groupe: Restructuration du projet</t>
   </si>
 </sst>
 </file>
@@ -608,7 +608,7 @@
   <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="2" spans="1:4" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="19"/>
     </row>
@@ -652,7 +652,7 @@
         <v>43153</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C5" s="10">
         <v>3</v>
@@ -663,7 +663,7 @@
         <v>43154</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C6" s="10">
         <v>2</v>
@@ -674,7 +674,7 @@
         <v>43160</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C7" s="10">
         <v>2</v>
@@ -685,7 +685,7 @@
         <v>43162</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="C8" s="10">
         <v>2</v>
@@ -696,7 +696,7 @@
         <v>43165</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="C9" s="10">
         <v>2</v>
@@ -707,7 +707,7 @@
         <v>43167</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10" s="10">
         <v>1</v>
@@ -718,7 +718,7 @@
         <v>43167</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="C11" s="10">
         <v>2</v>
@@ -741,7 +741,7 @@
         <v>43176</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C13" s="10">
         <v>2.5</v>
@@ -752,7 +752,7 @@
         <v>43179</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C14" s="10">
         <v>2</v>
@@ -763,7 +763,7 @@
         <v>43183</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C15" s="10">
         <v>8</v>
@@ -774,7 +774,7 @@
         <v>43186</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C16" s="10">
         <v>2</v>
@@ -785,7 +785,7 @@
         <v>43189</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C17" s="10">
         <v>4</v>
@@ -796,7 +796,7 @@
         <v>43193</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C18" s="10">
         <v>2</v>
@@ -809,7 +809,7 @@
         <v>43197</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C19" s="10">
         <v>6</v>
@@ -820,7 +820,7 @@
         <v>43200</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="C20" s="10">
         <v>2</v>
@@ -831,7 +831,7 @@
         <v>43204</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C21" s="10">
         <v>4</v>
@@ -842,7 +842,7 @@
         <v>43205</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C22" s="10">
         <v>3</v>
@@ -875,7 +875,7 @@
         <v>43215</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C25" s="10">
         <v>2</v>
@@ -886,7 +886,7 @@
         <v>43223</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C26" s="10">
         <v>2</v>
@@ -897,7 +897,7 @@
         <v>43228</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C27" s="10">
         <v>2</v>
@@ -908,7 +908,7 @@
         <v>43233</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C28" s="10">
         <v>2</v>
@@ -919,7 +919,7 @@
         <v>43235</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C29" s="10">
         <v>4</v>
@@ -932,7 +932,7 @@
         <v>43238</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C30" s="10">
         <v>6</v>
@@ -943,7 +943,7 @@
         <v>43239</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C31" s="10">
         <v>2</v>
@@ -954,7 +954,7 @@
         <v>43240</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C32" s="10">
         <v>6</v>
@@ -965,7 +965,7 @@
         <v>43241</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="C33" s="10">
         <v>2</v>
@@ -973,10 +973,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C34" s="10">
         <v>10</v>
@@ -984,10 +984,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C35" s="10">
         <v>8</v>
@@ -998,7 +998,7 @@
         <v>43244</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C36" s="10">
         <v>2</v>

</xml_diff>